<commit_message>
aggiunta link ai corsi
</commit_message>
<xml_diff>
--- a/DIETI_2023_24.xlsx
+++ b/DIETI_2023_24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcomaffeo/Desktop/GitHub/Erasmus-2023-24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanoriccardi/Desktop/UninaCorse/Erasmus-2023-24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CCEE0F-F6B6-6842-BF00-B80302E53AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4823AD62-5FAC-3A40-B98D-1F515F56B854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="163">
   <si>
     <r>
       <rPr>
@@ -279,27 +279,7 @@
         <rFont val="Calibri"/>
         <family val="1"/>
       </rPr>
-      <t>Engineering and engineering trades</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
       <t>Forestiere Carlo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>B2 English (certificato). a certificate of knowledge of English (B2-C1) written by university staff, preferably your English teacher, OR a score report of one of the following language tests: TOEFL (Test of English as a Foreign Language) - 92/iBT (incl. S</t>
     </r>
   </si>
   <si>
@@ -1546,6 +1526,24 @@
   </si>
   <si>
     <t>https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;cad=rja&amp;uact=8&amp;ved=2ahUKEwilus6_1cL9AhUPXvEDHW9mCvkQFnoECAoQAQ&amp;url=https%3A%2F%2Fwww.cranfield.ac.uk%2F&amp;usg=AOvVaw0U4-5B8-InNmYKjfvBP79g</t>
+  </si>
+  <si>
+    <t>B2 English (certificato). a certificate of knowledge of English (B2-C1) written by university staff, preferably your English teacher, OR a score report of one of the following language tests: TOEFL (Test of English as a Foreign Language) - 92/iBT (incl. S</t>
+  </si>
+  <si>
+    <t>Engineering and engineering trades</t>
+  </si>
+  <si>
+    <t>https://campus.tum.de/tumonline/ee/ui/ca2/app/desktop/#/pl/ui/$ctx/wbstpcs.showSpoTree?$ctx=design=ca2;header=max;lang=en&amp;pSJNr=1611&amp;pStStudiumNr=&amp;pStartSemester=&amp;pStpStpNr=4824</t>
+  </si>
+  <si>
+    <t>https://campus.tum.de/tumonline/ee/ui/ca2/app/desktop/#/pl/ui/$ctx/wbModHb.wbShow?$ctx=design=ca2;header=max;lang=en&amp;pOrgNr=14188</t>
+  </si>
+  <si>
+    <t>Corsi_KIT.pdf</t>
+  </si>
+  <si>
+    <t>belgio_inutile.png</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1554,7 @@
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1759,7 +1757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1946,6 +1944,48 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1964,47 +2004,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2344,14 +2348,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="11.19921875" customWidth="1"/>
     <col min="2" max="2" width="17.19921875" customWidth="1"/>
@@ -2362,25 +2366,27 @@
     <col min="7" max="7" width="26.59765625" customWidth="1"/>
     <col min="8" max="8" width="25.796875" customWidth="1"/>
     <col min="12" max="12" width="25.796875" customWidth="1"/>
+    <col min="13" max="13" width="28.19921875" customWidth="1"/>
+    <col min="14" max="14" width="24.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="68" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="69"/>
-    </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="20.25" customHeight="1">
+      <c r="A1" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="62"/>
+    </row>
+    <row r="2" spans="1:14" ht="20.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2403,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
@@ -2414,16 +2420,16 @@
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="70" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="55.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L2" s="63" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="68" customHeight="1">
       <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>13</v>
@@ -2452,19 +2458,22 @@
       <c r="K3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="73" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="74.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L3" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="M3" s="82" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="74.5" customHeight="1">
       <c r="A4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>21</v>
+      <c r="C4" s="68" t="s">
+        <v>158</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -2473,13 +2482,13 @@
         <v>9</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>20</v>
@@ -2490,19 +2499,19 @@
       <c r="K4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="73" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L4" s="66" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="27.75" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="72" t="s">
-        <v>124</v>
+        <v>23</v>
+      </c>
+      <c r="B5" s="65" t="s">
+        <v>122</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="9">
         <v>2</v>
@@ -2511,16 +2520,16 @@
         <v>5</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>36</v>
-      </c>
       <c r="I5" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J5" s="11">
         <v>61</v>
@@ -2528,19 +2537,19 @@
       <c r="K5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="73" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L5" s="66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="66" customHeight="1">
       <c r="A6" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="72" t="s">
-        <v>126</v>
+        <v>116</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>124</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="9">
         <v>2</v>
@@ -2549,36 +2558,39 @@
         <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J6" s="23">
         <v>61</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="73" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="37.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>38</v>
+      </c>
+      <c r="L6" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="M6" s="82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="37.25" customHeight="1">
       <c r="A7" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="71" t="s">
-        <v>128</v>
+        <v>36</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>126</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" s="19">
         <v>2</v>
@@ -2587,36 +2599,36 @@
         <v>10</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="73" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="55.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="74" t="s">
-        <v>130</v>
+      <c r="L7" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="55.75" customHeight="1">
+      <c r="A8" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>128</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
@@ -2628,33 +2640,33 @@
         <v>11</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J8" s="22">
         <v>713</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="73" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="L8" s="66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="63" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="72" t="s">
-        <v>132</v>
+        <v>36</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>130</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="9">
         <v>2</v>
@@ -2663,16 +2675,16 @@
         <v>10</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="I9" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J9" s="22">
         <v>713</v>
@@ -2680,19 +2692,25 @@
       <c r="K9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="73" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L9" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="M9" s="83" t="s">
+        <v>159</v>
+      </c>
+      <c r="N9" s="83" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="27.75" customHeight="1">
       <c r="A10" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B10" s="71" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="D10" s="9">
         <v>2</v>
@@ -2701,16 +2719,16 @@
         <v>5</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J10" s="24">
         <v>71</v>
@@ -2718,19 +2736,19 @@
       <c r="K10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="73" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="55.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L10" s="66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="55.75" customHeight="1">
       <c r="A11" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="75" t="s">
-        <v>136</v>
+        <v>62</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>134</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11" s="9">
         <v>2</v>
@@ -2739,33 +2757,33 @@
         <v>5</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J11" s="24">
         <v>61</v>
       </c>
       <c r="K11" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" s="73" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+      <c r="L11" s="66" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="46.5" customHeight="1">
       <c r="A12" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="71" t="s">
-        <v>138</v>
+        <v>72</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>136</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>13</v>
@@ -2777,36 +2795,36 @@
         <v>5</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J12" s="8">
         <v>714</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="73" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="L12" s="66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="46.5" customHeight="1">
       <c r="A13" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>140</v>
+        <v>77</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>138</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" s="9">
         <v>3</v>
@@ -2815,36 +2833,36 @@
         <v>5</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>80</v>
-      </c>
       <c r="J13" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="73" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L13" s="66" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="27.75" customHeight="1">
       <c r="A14" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D14" s="9">
         <v>4</v>
@@ -2853,36 +2871,36 @@
         <v>5</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="I14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="66" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="27.75" customHeight="1">
+      <c r="A15" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="K14" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="73" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="72" t="s">
-        <v>96</v>
+      <c r="B15" s="65" t="s">
+        <v>94</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="9">
         <v>3</v>
@@ -2891,36 +2909,36 @@
         <v>9</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J15" s="24">
         <v>714</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" s="76" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="55.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="L15" s="69" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="55.75" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="9">
         <v>2</v>
@@ -2929,16 +2947,16 @@
         <v>9</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J16" s="25">
         <v>713</v>
@@ -2946,16 +2964,16 @@
       <c r="K16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="73" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L16" s="66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="46.5" customHeight="1">
       <c r="A17" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="72" t="s">
-        <v>147</v>
+        <v>89</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>145</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>13</v>
@@ -2967,16 +2985,16 @@
         <v>9</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J17" s="25">
         <v>714</v>
@@ -2984,19 +3002,19 @@
       <c r="K17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L17" s="73" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L17" s="66" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="27.75" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="71" t="s">
-        <v>149</v>
+        <v>89</v>
+      </c>
+      <c r="B18" s="64" t="s">
+        <v>147</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="9">
         <v>1</v>
@@ -3005,36 +3023,36 @@
         <v>5</v>
       </c>
       <c r="F18" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>107</v>
-      </c>
       <c r="I18" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J18" s="11">
         <v>714</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L18" s="73" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="L18" s="66" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="27.75" customHeight="1">
       <c r="A19" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="77" t="s">
-        <v>151</v>
+        <v>106</v>
+      </c>
+      <c r="B19" s="70" t="s">
+        <v>149</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" s="53">
         <v>2</v>
@@ -3043,16 +3061,16 @@
         <v>9</v>
       </c>
       <c r="F19" s="54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H19" s="55" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I19" s="54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J19" s="56">
         <v>714</v>
@@ -3060,19 +3078,19 @@
       <c r="K19" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="L19" s="78" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L19" s="71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="65" customHeight="1">
       <c r="A20" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20" s="9">
         <v>2</v>
@@ -3081,16 +3099,16 @@
         <v>5</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J20" s="8">
         <v>714</v>
@@ -3098,19 +3116,19 @@
       <c r="K20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="73" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="126" x14ac:dyDescent="0.15">
+      <c r="L20" s="66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="126">
       <c r="A21" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="79" t="s">
-        <v>155</v>
+        <v>52</v>
+      </c>
+      <c r="B21" s="72" t="s">
+        <v>153</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="38">
         <v>4</v>
@@ -3119,33 +3137,33 @@
         <v>5</v>
       </c>
       <c r="F21" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="40" t="s">
-        <v>63</v>
-      </c>
       <c r="I21" s="41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J21" s="42">
         <v>533</v>
       </c>
       <c r="K21" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="L21" s="80" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="126" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+      <c r="L21" s="73" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="126">
       <c r="A22" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="81" t="s">
-        <v>157</v>
+        <v>62</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>155</v>
       </c>
       <c r="C22" s="44" t="s">
         <v>13</v>
@@ -3157,25 +3175,25 @@
         <v>5</v>
       </c>
       <c r="F22" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" s="37" t="s">
-        <v>69</v>
-      </c>
       <c r="I22" s="47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J22" s="48">
         <v>714</v>
       </c>
       <c r="K22" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="L22" s="80" t="s">
-        <v>158</v>
+        <v>64</v>
+      </c>
+      <c r="L22" s="73" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3203,8 +3221,13 @@
     <hyperlink ref="L20" r:id="rId18" xr:uid="{E0FDFFDA-B4C6-0843-9F63-7E07C6FF029C}"/>
     <hyperlink ref="L21" r:id="rId19" xr:uid="{972F9AF7-15F2-7C4C-9464-DD5FF8D44825}"/>
     <hyperlink ref="L22" r:id="rId20" xr:uid="{B48ABD11-A59F-3B4F-9907-B8EA0CF0E5E8}"/>
+    <hyperlink ref="N9" r:id="rId21" location="/pl/ui/$ctx/wbModHb.wbShow?$ctx=design=ca2;header=max;lang=en&amp;pOrgNr=14188" xr:uid="{336DC764-2909-1E42-BB92-95AA301307BE}"/>
+    <hyperlink ref="M9" r:id="rId22" location="/pl/ui/$ctx/wbstpcs.showSpoTree?$ctx=design=ca2;header=max;lang=en&amp;pSJNr=1611&amp;pStStudiumNr=&amp;pStartSemester=&amp;pStpStpNr=4824" xr:uid="{F524B646-16AF-C845-B9E1-7B818EEFFFD5}"/>
+    <hyperlink ref="M6" r:id="rId23" xr:uid="{D5CA5A5A-F7C2-5F4E-964F-3891ABAA2F7E}"/>
+    <hyperlink ref="M3" r:id="rId24" xr:uid="{711FC1B2-7FEA-DE42-93AC-42ED0222948D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -3216,7 +3239,7 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="11.19921875" customWidth="1"/>
     <col min="2" max="2" width="28.59765625" customWidth="1"/>
@@ -3224,113 +3247,113 @@
     <col min="6" max="6" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="9.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="63" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="69"/>
-    </row>
-    <row r="2" spans="1:12" ht="9.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
+    <row r="1" spans="1:12" ht="9.25" customHeight="1">
+      <c r="A1" s="77" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="62"/>
+    </row>
+    <row r="2" spans="1:12" ht="9.25" customHeight="1">
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
       <c r="C2" s="50"/>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I2" s="15"/>
       <c r="L2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="9.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="65"/>
-      <c r="B3" s="64"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="9.25" customHeight="1">
+      <c r="A3" s="79"/>
+      <c r="B3" s="78"/>
       <c r="E3" s="31"/>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="66"/>
-      <c r="B4" s="67"/>
+    <row r="4" spans="1:12" ht="17.25" customHeight="1">
+      <c r="A4" s="80"/>
+      <c r="B4" s="81"/>
       <c r="E4" s="31"/>
       <c r="I4" s="28"/>
     </row>
-    <row r="5" spans="1:12" ht="9.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="9.25" customHeight="1">
       <c r="A5" s="30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E5" s="31"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12">
       <c r="A6" s="31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E6" s="31"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12">
       <c r="A7" s="31"/>
       <c r="E7" s="31"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12">
       <c r="A8" s="31"/>
       <c r="E8" s="31"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12">
       <c r="A9" s="31"/>
       <c r="E9" s="31"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12">
       <c r="A10" s="31"/>
       <c r="E10" s="31"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12">
       <c r="A11" s="31"/>
       <c r="E11" s="31"/>
       <c r="K11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="31"/>
       <c r="E12" s="31"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12">
       <c r="A13" s="31"/>
       <c r="E13" s="31"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12">
       <c r="A14" s="31"/>
       <c r="E14" s="31"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12">
       <c r="A15" s="31"/>
       <c r="E15" s="31"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12">
       <c r="A16" s="31"/>
       <c r="E16" s="31"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12">
       <c r="A17" s="31"/>
       <c r="E17" s="31"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12">
       <c r="A18" s="31"/>
       <c r="E18" s="31"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12">
       <c r="A19" s="57"/>
       <c r="B19" s="57"/>
       <c r="C19" s="57"/>
@@ -3344,11 +3367,11 @@
       <c r="K19" s="57"/>
       <c r="L19" s="57"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12">
       <c r="A20" s="31"/>
       <c r="E20" s="31"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12">
       <c r="A21" s="49"/>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
@@ -3362,7 +3385,7 @@
       <c r="K21" s="49"/>
       <c r="L21" s="49"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12">
       <c r="A22" s="49"/>
       <c r="B22" s="49"/>
       <c r="C22" s="49"/>

</xml_diff>